<commit_message>
change for a new week
</commit_message>
<xml_diff>
--- a/excels/week1/bookPt.xlsx
+++ b/excels/week1/bookPt.xlsx
@@ -2,50 +2,425 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
+  <workbookPr defaultThemeVersion="164011"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\дом\Desktop\Рома\Расписание\servers\raspServer\Последняя версия проектаv2.0\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12345"/>
   </bookViews>
   <sheets>
     <sheet name="1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
-  <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
-      <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-  </extLst>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1" uniqueCount="1">
-  <si>
-    <t>Изменений на этот день нет</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="20">
+  <si>
+    <t>Ii смена</t>
+  </si>
+  <si>
+    <t>№</t>
+  </si>
+  <si>
+    <t>Время</t>
+  </si>
+  <si>
+    <t>7а</t>
+  </si>
+  <si>
+    <t>7б</t>
+  </si>
+  <si>
+    <t>7в</t>
+  </si>
+  <si>
+    <t>13:40 - 14:15</t>
+  </si>
+  <si>
+    <t>География</t>
+  </si>
+  <si>
+    <t>Русский язык</t>
+  </si>
+  <si>
+    <t>14:30 - 15:05</t>
+  </si>
+  <si>
+    <t>Физическая культура</t>
+  </si>
+  <si>
+    <t>15:20 - 15:55</t>
+  </si>
+  <si>
+    <t>16:10 - 16:45</t>
+  </si>
+  <si>
+    <t>17:00 - 17:35</t>
+  </si>
+  <si>
+    <t>17:50 - 18:25</t>
+  </si>
+  <si>
+    <t>18:30 - 19:05</t>
+  </si>
+  <si>
+    <t>Изменения на 20.05 (пятница)</t>
+  </si>
+  <si>
+    <t>Пятница</t>
+  </si>
+  <si>
+    <t>Физика</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <charset val="204"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="204"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri Light"/>
+      <family val="2"/>
+      <charset val="204"/>
+      <scheme val="major"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="204"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="204"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="204"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="204"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="204"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="204"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="204"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="204"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="204"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="204"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="204"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="204"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="204"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="204"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="204"/>
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="33">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.79998168889431442"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.59999389629810485"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.39997558519241921"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.79998168889431442"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.59999389629810485"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.39997558519241921"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.79998168889431442"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.59999389629810485"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.39997558519241921"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.79998168889431442"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.59999389629810485"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.39997558519241921"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.79998168889431442"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.59999389629810485"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.39997558519241921"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.79998168889431442"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.59999389629810485"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.39997558519241921"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="10">
     <border>
       <left/>
       <right/>
@@ -53,15 +428,204 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thick">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thick">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.39997558519241921"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="5" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="6" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="6" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="7" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="8" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="42">
+    <cellStyle name="20% — акцент1" xfId="19" builtinId="30" customBuiltin="1"/>
+    <cellStyle name="20% — акцент2" xfId="23" builtinId="34" customBuiltin="1"/>
+    <cellStyle name="20% — акцент3" xfId="27" builtinId="38" customBuiltin="1"/>
+    <cellStyle name="20% — акцент4" xfId="31" builtinId="42" customBuiltin="1"/>
+    <cellStyle name="20% — акцент5" xfId="35" builtinId="46" customBuiltin="1"/>
+    <cellStyle name="20% — акцент6" xfId="39" builtinId="50" customBuiltin="1"/>
+    <cellStyle name="40% — акцент1" xfId="20" builtinId="31" customBuiltin="1"/>
+    <cellStyle name="40% — акцент2" xfId="24" builtinId="35" customBuiltin="1"/>
+    <cellStyle name="40% — акцент3" xfId="28" builtinId="39" customBuiltin="1"/>
+    <cellStyle name="40% — акцент4" xfId="32" builtinId="43" customBuiltin="1"/>
+    <cellStyle name="40% — акцент5" xfId="36" builtinId="47" customBuiltin="1"/>
+    <cellStyle name="40% — акцент6" xfId="40" builtinId="51" customBuiltin="1"/>
+    <cellStyle name="60% — акцент1" xfId="21" builtinId="32" customBuiltin="1"/>
+    <cellStyle name="60% — акцент2" xfId="25" builtinId="36" customBuiltin="1"/>
+    <cellStyle name="60% — акцент3" xfId="29" builtinId="40" customBuiltin="1"/>
+    <cellStyle name="60% — акцент4" xfId="33" builtinId="44" customBuiltin="1"/>
+    <cellStyle name="60% — акцент5" xfId="37" builtinId="48" customBuiltin="1"/>
+    <cellStyle name="60% — акцент6" xfId="41" builtinId="52" customBuiltin="1"/>
+    <cellStyle name="Акцент1" xfId="18" builtinId="29" customBuiltin="1"/>
+    <cellStyle name="Акцент2" xfId="22" builtinId="33" customBuiltin="1"/>
+    <cellStyle name="Акцент3" xfId="26" builtinId="37" customBuiltin="1"/>
+    <cellStyle name="Акцент4" xfId="30" builtinId="41" customBuiltin="1"/>
+    <cellStyle name="Акцент5" xfId="34" builtinId="45" customBuiltin="1"/>
+    <cellStyle name="Акцент6" xfId="38" builtinId="49" customBuiltin="1"/>
+    <cellStyle name="Ввод " xfId="9" builtinId="20" customBuiltin="1"/>
+    <cellStyle name="Вывод" xfId="10" builtinId="21" customBuiltin="1"/>
+    <cellStyle name="Вычисление" xfId="11" builtinId="22" customBuiltin="1"/>
+    <cellStyle name="Заголовок 1" xfId="2" builtinId="16" customBuiltin="1"/>
+    <cellStyle name="Заголовок 2" xfId="3" builtinId="17" customBuiltin="1"/>
+    <cellStyle name="Заголовок 3" xfId="4" builtinId="18" customBuiltin="1"/>
+    <cellStyle name="Заголовок 4" xfId="5" builtinId="19" customBuiltin="1"/>
+    <cellStyle name="Итог" xfId="17" builtinId="25" customBuiltin="1"/>
+    <cellStyle name="Контрольная ячейка" xfId="13" builtinId="23" customBuiltin="1"/>
+    <cellStyle name="Название" xfId="1" builtinId="15" customBuiltin="1"/>
+    <cellStyle name="Нейтральный" xfId="8" builtinId="28" customBuiltin="1"/>
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
+    <cellStyle name="Плохой" xfId="7" builtinId="27" customBuiltin="1"/>
+    <cellStyle name="Пояснение" xfId="16" builtinId="53" customBuiltin="1"/>
+    <cellStyle name="Примечание" xfId="15" builtinId="10" customBuiltin="1"/>
+    <cellStyle name="Связанная ячейка" xfId="12" builtinId="24" customBuiltin="1"/>
+    <cellStyle name="Текст предупреждения" xfId="14" builtinId="11" customBuiltin="1"/>
+    <cellStyle name="Хороший" xfId="6" builtinId="26" customBuiltin="1"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -339,17 +903,197 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:I10"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="J3" sqref="J3:M7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="30.140625" customWidth="1"/>
+    <col min="2" max="2" width="33.28515625" customWidth="1"/>
+    <col min="3" max="3" width="16.140625" customWidth="1"/>
+    <col min="4" max="4" width="21.28515625" customWidth="1"/>
+    <col min="6" max="6" width="17.140625" customWidth="1"/>
+    <col min="7" max="7" width="9" customWidth="1"/>
+    <col min="8" max="8" width="24" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
         <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D3" t="s">
+        <v>3</v>
+      </c>
+      <c r="F3" t="s">
+        <v>4</v>
+      </c>
+      <c r="H3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>17</v>
+      </c>
+      <c r="B4">
+        <v>0</v>
+      </c>
+      <c r="C4" t="s">
+        <v>6</v>
+      </c>
+      <c r="D4" t="s">
+        <v>18</v>
+      </c>
+      <c r="E4">
+        <v>10</v>
+      </c>
+      <c r="F4" t="s">
+        <v>10</v>
+      </c>
+      <c r="G4">
+        <v>7</v>
+      </c>
+      <c r="H4" t="s">
+        <v>8</v>
+      </c>
+      <c r="I4">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B5">
+        <v>1</v>
+      </c>
+      <c r="C5" t="s">
+        <v>9</v>
+      </c>
+      <c r="D5" t="s">
+        <v>7</v>
+      </c>
+      <c r="E5">
+        <v>10</v>
+      </c>
+      <c r="F5" t="s">
+        <v>10</v>
+      </c>
+      <c r="G5" t="s">
+        <v>19</v>
+      </c>
+      <c r="H5" t="s">
+        <v>18</v>
+      </c>
+      <c r="I5">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B6">
+        <v>2</v>
+      </c>
+      <c r="C6" t="s">
+        <v>11</v>
+      </c>
+      <c r="D6" t="s">
+        <v>7</v>
+      </c>
+      <c r="E6">
+        <v>10</v>
+      </c>
+      <c r="F6" t="s">
+        <v>18</v>
+      </c>
+      <c r="G6">
+        <v>7</v>
+      </c>
+      <c r="H6" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B7">
+        <v>3</v>
+      </c>
+      <c r="C7" t="s">
+        <v>12</v>
+      </c>
+      <c r="D7" t="s">
+        <v>19</v>
+      </c>
+      <c r="E7" t="s">
+        <v>19</v>
+      </c>
+      <c r="G7">
+        <v>7</v>
+      </c>
+      <c r="H7" t="s">
+        <v>10</v>
+      </c>
+      <c r="I7">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B8">
+        <v>4</v>
+      </c>
+      <c r="C8" t="s">
+        <v>13</v>
+      </c>
+      <c r="D8" t="s">
+        <v>19</v>
+      </c>
+      <c r="E8" t="s">
+        <v>19</v>
+      </c>
+      <c r="G8" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B9">
+        <v>5</v>
+      </c>
+      <c r="C9" t="s">
+        <v>14</v>
+      </c>
+      <c r="D9" t="s">
+        <v>19</v>
+      </c>
+      <c r="E9" t="s">
+        <v>19</v>
+      </c>
+      <c r="G9" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B10">
+        <v>6</v>
+      </c>
+      <c r="C10" t="s">
+        <v>15</v>
+      </c>
+      <c r="D10" t="s">
+        <v>19</v>
+      </c>
+      <c r="E10" t="s">
+        <v>19</v>
       </c>
     </row>
   </sheetData>

</xml_diff>